<commit_message>
minor changes to some xlsx tables and nfishers data almost complete
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb125/raw/Table4.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb125/raw/Table4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb125/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E173541-77DC-604F-8E45-FE8C5CD08FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FE0FBE-A48F-FA41-99EA-D0EF6CF83F6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Area of residence</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Total check</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
   </si>
 </sst>
 </file>
@@ -80,7 +83,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -157,19 +160,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -488,17 +491,17 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="52"/>
     <col min="2" max="2" width="16"/>
     <col min="3" max="3" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,8 +567,10 @@
         <v>706</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B7" s="6">
         <v>2287</v>
       </c>

</xml_diff>